<commit_message>
Improve formatting for '漢字' type questions in PDF
Updated create_pdf.py to parse and format '漢字' type questions using regex, allowing for bolded segments within the question text. Adjusted line spacing for better readability and improved the layout of question numbering and text.
</commit_message>
<xml_diff>
--- a/soal.xlsx
+++ b/soal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fariz Armesta\Documents\GitHub\test-maker-jp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D034645-4EC0-4999-95DF-940A86266F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96747CC7-1DDE-454B-A10B-D2F534C782B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="15">
   <si>
     <t>案内</t>
   </si>
@@ -42,7 +42,7 @@
     <t>漢字</t>
   </si>
   <si>
-    <t>彼は今、新薬の研究開発に・挑んで・いる。</t>
+    <t>彼は今、新薬の研究開発に|挑んで|いる。</t>
   </si>
   <si>
     <t>はげんで</t>
@@ -57,7 +57,7 @@
     <t>いどんで</t>
   </si>
   <si>
-    <t>住民が建設会社を相手に、・訴訟・を起こした。</t>
+    <t>住民が建設会社を相手に、|訴訟|を起こした。</t>
   </si>
   <si>
     <t>そしょう</t>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>問題２＿＿＿の言葉の読み方として最もよいものを、１・２・３・４から一つ選びなさい</t>
+  </si>
+  <si>
+    <t>彼は今、新薬の研究開発に|挑んで|いるうううううううううううううううううううううううううううううううううううううううう。</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
   <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -413,7 +416,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Add support for '白' type questions in PDF generator
Extended the PDFCreator class to handle questions of type '白', formatting them with Japanese font and displaying answer choices in four columns. Updated the output PDF and source Excel file accordingly.
</commit_message>
<xml_diff>
--- a/soal.xlsx
+++ b/soal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fariz Armesta\Documents\GitHub\test-maker-jp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96747CC7-1DDE-454B-A10B-D2F534C782B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FAE316-6429-45D5-B552-3CEBD81F6B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="21">
   <si>
     <t>案内</t>
   </si>
@@ -42,40 +42,58 @@
     <t>漢字</t>
   </si>
   <si>
+    <t>彼は今、新薬の研究開発に|挑んで|いるうううううううううううううううううううううううううううううううううううううううう。</t>
+  </si>
+  <si>
+    <t>はげんで</t>
+  </si>
+  <si>
+    <t>のぞんで</t>
+  </si>
+  <si>
+    <t>からんで</t>
+  </si>
+  <si>
+    <t>いどんで</t>
+  </si>
+  <si>
+    <t>住民が建設会社を相手に、|訴訟|を起こした。</t>
+  </si>
+  <si>
+    <t>そしょう</t>
+  </si>
+  <si>
+    <t>せきしょう</t>
+  </si>
+  <si>
+    <t>そこう</t>
+  </si>
+  <si>
+    <t>せっこう</t>
+  </si>
+  <si>
     <t>彼は今、新薬の研究開発に|挑んで|いる。</t>
   </si>
   <si>
-    <t>はげんで</t>
-  </si>
-  <si>
-    <t>のぞんで</t>
-  </si>
-  <si>
-    <t>からんで</t>
-  </si>
-  <si>
-    <t>いどんで</t>
-  </si>
-  <si>
-    <t>住民が建設会社を相手に、|訴訟|を起こした。</t>
-  </si>
-  <si>
-    <t>そしょう</t>
-  </si>
-  <si>
-    <t>せきしょう</t>
-  </si>
-  <si>
-    <t>そこう</t>
-  </si>
-  <si>
-    <t>せっこう</t>
-  </si>
-  <si>
-    <t>問題２＿＿＿の言葉の読み方として最もよいものを、１・２・３・４から一つ選びなさい</t>
-  </si>
-  <si>
-    <t>彼は今、新薬の研究開発に|挑んで|いるうううううううううううううううううううううううううううううううううううううううう。</t>
+    <t>問題２　（　　　）に入れるのに最もよいものを、１・２・３・４から一つ選びなさい。</t>
+  </si>
+  <si>
+    <t>私は主張は単なる（　　）ではなく、確たる証拠に基づいている。</t>
+  </si>
+  <si>
+    <t>爆発</t>
+  </si>
+  <si>
+    <t>視線</t>
+  </si>
+  <si>
+    <t>推測</t>
+  </si>
+  <si>
+    <t>推移</t>
+  </si>
+  <si>
+    <t>白</t>
   </si>
 </sst>
 </file>
@@ -391,7 +409,7 @@
   <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -416,7 +434,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -456,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -496,7 +514,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -536,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -576,7 +594,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -616,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -656,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -696,127 +714,127 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>